<commit_message>
Completed NBA_model data set and saved as NBA_model.csv
</commit_message>
<xml_diff>
--- a/Dirty_Data/NBA_Index.xlsx
+++ b/Dirty_Data/NBA_Index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12812\Desktop\Final_Project\NBA_Scout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ovais\Desktop\Project-3\Dirty_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414ED2DC-87A4-4F5B-9AD3-2BE91C881230}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E86F00-F933-4554-979B-2BC2B2EC355E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E28D675C-0773-4068-B2C4-5EB03BB4EDB5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{E28D675C-0773-4068-B2C4-5EB03BB4EDB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>LAC</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>ORL</t>
-  </si>
-  <si>
-    <t>Orlando Magic</t>
   </si>
   <si>
     <t>BKN</t>
@@ -610,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B820AD9C-E5D2-4792-BC68-0E52545A5FDA}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +620,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,10 +636,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +687,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +703,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +711,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,7 +759,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,10 +788,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,15 +799,15 @@
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,42 +820,42 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>